<commit_message>
Invitation Task: Modified schedule. Added new schedules. Split module 3 into blocks and added scoring (bar and popup). Split module 2 into different parts (accept office, reject office, accept library, reject library). Various aesthetic changes.
</commit_message>
<xml_diff>
--- a/public/js/tasks/invitation_task/MCQ_mapping_module3-2.xlsx
+++ b/public/js/tasks/invitation_task/MCQ_mapping_module3-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtouthang/iCloud Drive (Archive)/Documents/Documents - L00019188/StimTool_Online/public/js/tasks/invitation_task/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARobinson\Documents\stimtool\stimtool_schedules\invitation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC55B7B1-5BB5-3447-8F22-CCC0A1818212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBDB12F-7264-42A5-A48A-296B02AFC313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21360" windowHeight="16960" xr2:uid="{193BAE17-2DD3-4B9C-A546-95C76A9087F0}"/>
+    <workbookView xWindow="5445" yWindow="-12405" windowWidth="21600" windowHeight="11835" xr2:uid="{193BAE17-2DD3-4B9C-A546-95C76A9087F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="34">
   <si>
     <t>building_type</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>path_version</t>
+  </si>
+  <si>
+    <t>20-20</t>
+  </si>
+  <si>
+    <t>10-25</t>
   </si>
 </sst>
 </file>
@@ -483,19 +489,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E664A047-A8AA-4A90-B33E-4BBE354FFB25}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" customWidth="1"/>
-    <col min="5" max="8" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="5" max="8" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -527,7 +533,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -550,7 +556,7 @@
         <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>10</v>
@@ -559,7 +565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -579,7 +585,7 @@
         <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>15</v>
@@ -591,7 +597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -611,7 +617,7 @@
         <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>13</v>
@@ -623,7 +629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -637,7 +643,7 @@
         <v>29</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
@@ -655,7 +661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -669,7 +675,7 @@
         <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>21</v>
@@ -687,7 +693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -707,7 +713,7 @@
         <v>11</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>21</v>
@@ -719,7 +725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -736,7 +742,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
@@ -751,7 +757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -765,7 +771,7 @@
         <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>16</v>
@@ -783,7 +789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -800,7 +806,7 @@
         <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>21</v>
@@ -815,7 +821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -829,10 +835,10 @@
         <v>29</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>25</v>
@@ -847,7 +853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -867,7 +873,7 @@
         <v>17</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>16</v>
@@ -879,7 +885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -896,7 +902,7 @@
         <v>18</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>16</v>
@@ -911,7 +917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -934,7 +940,7 @@
         <v>18</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>10</v>
@@ -943,7 +949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -960,10 +966,10 @@
         <v>19</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>12</v>
@@ -975,7 +981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -995,7 +1001,7 @@
         <v>26</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>15</v>
@@ -1007,7 +1013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1021,7 +1027,7 @@
         <v>29</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>17</v>
@@ -1039,7 +1045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1071,7 +1077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1091,7 +1097,7 @@
         <v>18</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>15</v>
@@ -1103,7 +1109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1123,7 @@
         <v>30</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>13</v>
@@ -1135,7 +1141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1155,7 +1161,7 @@
         <v>21</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>18</v>
@@ -1167,7 +1173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1181,7 +1187,7 @@
         <v>30</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>15</v>
@@ -1199,7 +1205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -1213,7 +1219,7 @@
         <v>29</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>14</v>
@@ -1231,7 +1237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1254,7 +1260,7 @@
         <v>21</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>10</v>
@@ -1263,7 +1269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -1277,7 +1283,7 @@
         <v>29</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>26</v>
@@ -1295,7 +1301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1315,7 +1321,7 @@
         <v>20</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>15</v>
@@ -1327,7 +1333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1350,7 +1356,7 @@
         <v>14</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>10</v>
@@ -1359,7 +1365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -1373,10 +1379,10 @@
         <v>30</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>20</v>
@@ -1391,7 +1397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1405,7 +1411,7 @@
         <v>29</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>19</v>

</xml_diff>